<commit_message>
update sql & comleted DetailStudentInformation
</commit_message>
<xml_diff>
--- a/course.xlsx
+++ b/course.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Desktop\StudentManagement\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\JavaProject\StudentManagement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA8B68A0-7A60-4824-B193-A178C781B9F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{049A0363-D851-426F-9FF2-52EAA926219F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D93DEF0E-9E5E-4CFD-83AA-8A37395EBFAD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D93DEF0E-9E5E-4CFD-83AA-8A37395EBFAD}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>K01</t>
   </si>
@@ -61,13 +61,31 @@
   </si>
   <si>
     <t>JAVA SWING</t>
+  </si>
+  <si>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Start time</t>
+  </si>
+  <si>
+    <t>End time</t>
+  </si>
+  <si>
+    <t>grade Quantity</t>
+  </si>
+  <si>
+    <t>Cost</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -76,37 +94,21 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF333333"/>
-      <name val="Arial"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -114,61 +116,20 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-    </font>
   </fonts>
-  <fills count="5">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFEFF3FB"/>
-        <bgColor rgb="FFEFF3FB"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF1F0F0"/>
-        <bgColor rgb="FFF1F0F0"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="4">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000066"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color rgb="FF000066"/>
-      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -188,63 +149,34 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -556,205 +488,144 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{031DF760-193C-4C61-8773-5A05981EB4A4}">
-  <dimension ref="A1:J10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AD901F3-BC26-4278-91D2-B5F556C145B7}">
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19" customWidth="1"/>
-    <col min="2" max="2" width="23.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15.44140625" customWidth="1"/>
-    <col min="4" max="4" width="26.33203125" customWidth="1"/>
-    <col min="5" max="5" width="15.88671875" customWidth="1"/>
-    <col min="6" max="6" width="14.5546875" customWidth="1"/>
-    <col min="7" max="7" width="19" customWidth="1"/>
-    <col min="8" max="8" width="20.5546875" customWidth="1"/>
-    <col min="10" max="10" width="25.44140625" style="16" customWidth="1"/>
-    <col min="11" max="12" width="13.88671875" customWidth="1"/>
-    <col min="13" max="13" width="14.6640625" customWidth="1"/>
+    <col min="1" max="1" width="18.5703125" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" customWidth="1"/>
+    <col min="3" max="3" width="17" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" customWidth="1"/>
+    <col min="5" max="5" width="17" customWidth="1"/>
+    <col min="6" max="6" width="22.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1"/>
-      <c r="B1" s="2"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="5" t="s">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="18">
+      <c r="C2" s="5">
         <v>43911</v>
       </c>
-      <c r="H1" s="18">
+      <c r="D2" s="5">
         <v>44095</v>
       </c>
-      <c r="I1">
+      <c r="E2" s="2">
         <v>3</v>
       </c>
-      <c r="J1" s="17">
+      <c r="F2" s="6">
         <v>5000000</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="9"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="5" t="s">
+    <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="18">
+      <c r="C3" s="5">
         <v>43914</v>
       </c>
-      <c r="H2" s="18">
+      <c r="D3" s="5">
         <v>44098</v>
       </c>
-      <c r="I2">
+      <c r="E3" s="2">
         <v>2</v>
       </c>
-      <c r="J2" s="17">
+      <c r="F3" s="6">
         <v>4500000</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="11"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="13" t="s">
+    <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="18">
+      <c r="C4" s="5">
         <v>43923</v>
       </c>
-      <c r="H3" s="18">
+      <c r="D4" s="5">
         <v>44106</v>
       </c>
-      <c r="I3">
+      <c r="E4" s="2">
         <v>2</v>
       </c>
-      <c r="J3" s="17">
+      <c r="F4" s="6">
         <v>6000000</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="9"/>
-      <c r="B4" s="10"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="13" t="s">
+    <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="B5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="18">
+      <c r="C5" s="5">
         <v>43936</v>
       </c>
-      <c r="H4" s="18">
+      <c r="D5" s="5">
         <v>44119</v>
       </c>
-      <c r="I4">
+      <c r="E5" s="2">
         <v>3</v>
       </c>
-      <c r="J4" s="17">
+      <c r="F5" s="6">
         <v>5500000</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="11"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="5" t="s">
+    <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="B6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="18">
+      <c r="C6" s="5">
         <v>43946</v>
       </c>
-      <c r="H5" s="18">
+      <c r="D6" s="5">
         <v>44129</v>
       </c>
-      <c r="I5">
+      <c r="E6" s="2">
         <v>4</v>
       </c>
-      <c r="J5" s="17">
+      <c r="F6" s="6">
         <v>4000000</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="9"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="8"/>
-      <c r="J6" s="17"/>
-    </row>
-    <row r="7" spans="1:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="11"/>
-      <c r="B7" s="12"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="8"/>
-      <c r="J7" s="17"/>
-    </row>
-    <row r="8" spans="1:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="9"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="8"/>
-      <c r="J8" s="17"/>
-    </row>
-    <row r="9" spans="1:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="9"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="8"/>
-      <c r="J9" s="17"/>
-    </row>
-    <row r="10" spans="1:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="9"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="8"/>
-      <c r="J10" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>